<commit_message>
Added implementation of MSM measure.
</commit_message>
<xml_diff>
--- a/data/backend/forum-service_structure.xlsx
+++ b/data/backend/forum-service_structure.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10748" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10892" uniqueCount="508">
   <si>
     <t>Class Name</t>
   </si>
@@ -1029,27 +1029,27 @@
     <t>org.andante.forum.controller.TopicController</t>
   </si>
   <si>
+    <t>getTopic(java.lang.Long)</t>
+  </si>
+  <si>
+    <t>getHierarchy(java.lang.Long)</t>
+  </si>
+  <si>
+    <t>modify(dto.topic.TopicInputDTO)</t>
+  </si>
+  <si>
+    <t>getSubtopics(java.lang.Long)</t>
+  </si>
+  <si>
     <t>TopicController(org.andante.forum.logic.service.impl.TopicServiceImpl, org.andante.forum.controller.mapper.TopicDTOModelMapper, org.andante.mappers.OperationHttpStatusMapper)</t>
   </si>
   <si>
-    <t>getTopic(java.lang.Long)</t>
-  </si>
-  <si>
-    <t>getHierarchy(java.lang.Long)</t>
-  </si>
-  <si>
-    <t>modify(dto.topic.TopicInputDTO)</t>
-  </si>
-  <si>
     <t>getPage(dto.topic.TopicQuerySpecification)</t>
   </si>
   <si>
     <t>create(dto.topic.TopicInputDTO)</t>
   </si>
   <si>
-    <t>getSubtopics(java.lang.Long)</t>
-  </si>
-  <si>
     <t>delete(java.lang.Long)</t>
   </si>
   <si>
@@ -1062,6 +1062,9 @@
     <t>like(dto.post.PostLikeDTO)</t>
   </si>
   <si>
+    <t>modify(dto.post.PostInputDTO)</t>
+  </si>
+  <si>
     <t>create(dto.post.PostInputDTO)</t>
   </si>
   <si>
@@ -1069,9 +1072,6 @@
   </si>
   <si>
     <t>PostController(org.andante.forum.logic.service.impl.PostServiceImpl, org.andante.forum.controller.mapper.PostDTOModelMapper, org.andante.forum.controller.mapper.PostLikesDTOModelMapper, org.andante.mappers.OperationHttpStatusMapper)</t>
-  </si>
-  <si>
-    <t>modify(dto.post.PostInputDTO)</t>
   </si>
   <si>
     <t>org.andante.forum.controller.PostResponseController</t>
@@ -20158,7 +20158,7 @@
         <v>334</v>
       </c>
       <c r="B180" t="s" s="0">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C180" t="s" s="0">
         <v>458</v>
@@ -20169,7 +20169,7 @@
         <v>334</v>
       </c>
       <c r="B181" t="s" s="0">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C181" t="s" s="0">
         <v>485</v>
@@ -20180,7 +20180,7 @@
         <v>334</v>
       </c>
       <c r="B182" t="s" s="0">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C182" t="s" s="0">
         <v>485</v>
@@ -20202,7 +20202,7 @@
         <v>334</v>
       </c>
       <c r="B184" t="s" s="0">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C184" t="s" s="0">
         <v>485</v>
@@ -20213,7 +20213,7 @@
         <v>334</v>
       </c>
       <c r="B185" t="s" s="0">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C185" t="s" s="0">
         <v>458</v>
@@ -20224,7 +20224,7 @@
         <v>334</v>
       </c>
       <c r="B186" t="s" s="0">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C186" t="s" s="0">
         <v>458</v>
@@ -20246,7 +20246,7 @@
         <v>334</v>
       </c>
       <c r="B188" t="s" s="0">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C188" t="s" s="0">
         <v>458</v>
@@ -21434,7 +21434,7 @@
         <v>343</v>
       </c>
       <c r="B296" t="s" s="0">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C296" t="s" s="0">
         <v>458</v>
@@ -21478,7 +21478,7 @@
         <v>343</v>
       </c>
       <c r="B300" t="s" s="0">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C300" t="s" s="0">
         <v>458</v>
@@ -21500,7 +21500,7 @@
         <v>343</v>
       </c>
       <c r="B302" t="s" s="0">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C302" t="s" s="0">
         <v>458</v>
@@ -21522,7 +21522,7 @@
         <v>343</v>
       </c>
       <c r="B304" t="s" s="0">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C304" t="s" s="0">
         <v>478</v>
@@ -23293,7 +23293,7 @@
         <v>350</v>
       </c>
       <c r="B465" t="s" s="0">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C465" t="s" s="0">
         <v>458</v>
@@ -24692,7 +24692,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -24717,13 +24717,13 @@
         <v>334</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>335</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -24731,7 +24731,7 @@
         <v>334</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>6</v>
@@ -24745,7 +24745,7 @@
         <v>334</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>6</v>
@@ -24759,7 +24759,7 @@
         <v>334</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>6</v>
@@ -24773,13 +24773,13 @@
         <v>334</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>339</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>264</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
@@ -24787,7 +24787,7 @@
         <v>334</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C7" t="s" s="0">
         <v>6</v>
@@ -24801,13 +24801,13 @@
         <v>334</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>341</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>264</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
@@ -24829,63 +24829,63 @@
         <v>334</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>342</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>264</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>344</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>264</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>345</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>264</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="C13" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>264</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="C14" t="s" s="0">
         <v>6</v>
@@ -24896,10 +24896,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>192</v>
+        <v>341</v>
       </c>
       <c r="C15" t="s" s="0">
         <v>6</v>
@@ -24910,24 +24910,24 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>198</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D16" t="s" s="0">
-        <v>264</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>348</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s" s="0">
         <v>6</v>
@@ -24938,24 +24938,24 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>342</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D18" t="s" s="0">
-        <v>264</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>6</v>
@@ -24966,10 +24966,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="C20" t="s" s="0">
         <v>6</v>
@@ -24980,10 +24980,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="C21" t="s" s="0">
         <v>6</v>
@@ -24994,38 +24994,38 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>347</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>264</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>353</v>
+        <v>12</v>
       </c>
       <c r="C23" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>354</v>
+        <v>192</v>
       </c>
       <c r="C24" t="s" s="0">
         <v>6</v>
@@ -25036,38 +25036,38 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>355</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>264</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>342</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>264</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>356</v>
+        <v>343</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="C27" t="s" s="0">
         <v>6</v>
@@ -25078,44 +25078,548 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>356</v>
+        <v>343</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>358</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D28" t="s" s="0">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>356</v>
+        <v>343</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>133</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>264</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>356</v>
+        <v>343</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>136</v>
+        <v>347</v>
       </c>
       <c r="C30" t="s" s="0">
         <v>6</v>
       </c>
       <c r="D30" t="s" s="0">
         <v>264</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>348</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s" s="0">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>198</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s" s="0">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>349</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>343</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>342</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s" s="0">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>351</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s" s="0">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>352</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s" s="0">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>353</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>354</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>355</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>348</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>350</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>342</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D53" t="s" s="0">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>356</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>356</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>357</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D55" t="s" s="0">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>356</v>
+      </c>
+      <c r="B56" t="s" s="0">
+        <v>358</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>356</v>
+      </c>
+      <c r="B57" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C57" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D57" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>356</v>
+      </c>
+      <c r="B58" t="s" s="0">
+        <v>133</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s" s="0">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>356</v>
+      </c>
+      <c r="B59" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C59" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>356</v>
+      </c>
+      <c r="B60" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C60" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D60" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>356</v>
+      </c>
+      <c r="B61" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C61" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D61" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>356</v>
+      </c>
+      <c r="B62" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C62" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D62" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="0">
+        <v>356</v>
+      </c>
+      <c r="B63" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="C63" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D63" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="0">
+        <v>356</v>
+      </c>
+      <c r="B64" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C64" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D64" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="0">
+        <v>356</v>
+      </c>
+      <c r="B65" t="s" s="0">
+        <v>136</v>
+      </c>
+      <c r="C65" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D65" t="s" s="0">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="0">
+        <v>356</v>
+      </c>
+      <c r="B66" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C66" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D66" t="s" s="0">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -38607,7 +39111,7 @@
         <v>334</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>241</v>
@@ -38624,7 +39128,7 @@
         <v>334</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>290</v>
@@ -38658,7 +39162,7 @@
         <v>343</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>188</v>
@@ -38709,7 +39213,7 @@
         <v>334</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>290</v>
@@ -38794,7 +39298,7 @@
         <v>334</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C13" t="s" s="0">
         <v>290</v>
@@ -38811,7 +39315,7 @@
         <v>334</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C14" t="s" s="0">
         <v>290</v>
@@ -38862,7 +39366,7 @@
         <v>343</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C17" t="s" s="0">
         <v>188</v>
@@ -38896,7 +39400,7 @@
         <v>343</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>199</v>
@@ -38947,7 +39451,7 @@
         <v>334</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C22" t="s" s="0">
         <v>290</v>
@@ -38964,7 +39468,7 @@
         <v>350</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C23" t="s" s="0">
         <v>78</v>
@@ -38998,7 +39502,7 @@
         <v>343</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C25" t="s" s="0">
         <v>188</v>
@@ -39015,7 +39519,7 @@
         <v>343</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C26" t="s" s="0">
         <v>199</v>
@@ -39032,7 +39536,7 @@
         <v>350</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C27" t="s" s="0">
         <v>153</v>
@@ -39066,7 +39570,7 @@
         <v>334</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C29" t="s" s="0">
         <v>241</v>
@@ -39134,7 +39638,7 @@
         <v>334</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C33" t="s" s="0">
         <v>290</v>
@@ -39168,7 +39672,7 @@
         <v>334</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C35" t="s" s="0">
         <v>241</v>
@@ -39236,7 +39740,7 @@
         <v>343</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C39" t="s" s="0">
         <v>199</v>

</xml_diff>